<commit_message>
Move DH from DCs starting year to 2022
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SRV_DC_ExcessHeat.xlsx
+++ b/SubRES_TMPL/SubRES_SRV_DC_ExcessHeat.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4258797-E312-46F7-AAFF-2A1B6349A2DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FFC64B-53E6-4CCA-B859-609B6232E130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SRV_DC_Commodities" sheetId="11" r:id="rId1"/>
@@ -13,9 +13,6 @@
     <sheet name="HP_data" sheetId="14" r:id="rId3"/>
     <sheet name="HE_data" sheetId="15" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="DH_in_ex_app">HE_data!$C$8:$G$35</definedName>
     <definedName name="Elpriser">#REF!</definedName>
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="266">
   <si>
     <t>~FI_T</t>
   </si>
@@ -891,6 +888,51 @@
   </si>
   <si>
     <t>Source: Technology Data - Energy Plants for Electricity and District heating generation (V0009). Danish Energy Agency</t>
+  </si>
+  <si>
+    <t>Heat production capacity for one unit [kW_h]</t>
+  </si>
+  <si>
+    <t>Expected share of space heating demand covered by unit [p.u.]</t>
+  </si>
+  <si>
+    <t>Expected share of hot tap water demand covered by unit [p.u.]</t>
+  </si>
+  <si>
+    <t>Heat efficiency (annual average, net) [p.u.]</t>
+  </si>
+  <si>
+    <t>Auxiliary Electricity consumption [kWh_e/y]</t>
+  </si>
+  <si>
+    <t>Technical economic lifetime [years]</t>
+  </si>
+  <si>
+    <t>Primary regulation (per 30 seconds) [p.u.]</t>
+  </si>
+  <si>
+    <t>Secondary regulation (per minute) [p.u.]</t>
+  </si>
+  <si>
+    <t>Minimum load (of full load) [p.u.]</t>
+  </si>
+  <si>
+    <t>Warm start-up time [hours]</t>
+  </si>
+  <si>
+    <t>Cold start-up time [hours]</t>
+  </si>
+  <si>
+    <t>Fixed O&amp;M (*total) [€/unit/y, 2020]</t>
+  </si>
+  <si>
+    <t>Fixed O&amp;M (electricity cost) [€/unit/y, 2020]</t>
+  </si>
+  <si>
+    <t>Fixed O&amp;M (other) [€/unit/y, 2020]</t>
+  </si>
+  <si>
+    <t>Annual O&amp;M (time spent on manual maintenance) [hours/unit/y]</t>
   </si>
 </sst>
 </file>
@@ -1760,181 +1802,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Index"/>
-      <sheetName val="alldata_flat"/>
-      <sheetName val="201 Oil boiler, ex single"/>
-      <sheetName val="201 Oil boiler, ex apart"/>
-      <sheetName val="201 Oil boiler, new single"/>
-      <sheetName val="201 Oil boiler, new apart"/>
-      <sheetName val="202 Gas boiler, ex single"/>
-      <sheetName val="202 Gas boiler, ex apart"/>
-      <sheetName val="202 Gas boiler, new single"/>
-      <sheetName val="202 Gas boiler, new apart"/>
-      <sheetName val="203 DH indirect,new single"/>
-      <sheetName val="203 DH indirect,ex single"/>
-      <sheetName val="203 DH indirect,ex apart"/>
-      <sheetName val="203 DH indirect,new apart"/>
-      <sheetName val="203 DH direct,new single"/>
-      <sheetName val="203 DH direct,ex single"/>
-      <sheetName val="203 DH direct,ex apart"/>
-      <sheetName val="203 DH direct,new apart"/>
-      <sheetName val="204 Biomass auto,ex single"/>
-      <sheetName val="204 Biomass auto,new single"/>
-      <sheetName val="204 Biomass auto,ex apart"/>
-      <sheetName val="204 Biomass auto,new apart"/>
-      <sheetName val="205 Biomass manual,ex single"/>
-      <sheetName val="206 Wood stove,single, ex tank"/>
-      <sheetName val="206 Wood stove, single n w tank"/>
-      <sheetName val="207 HP air-water,ex single"/>
-      <sheetName val="207 HP air-water,ex apart"/>
-      <sheetName val="207 HP air-water LPP,ex single"/>
-      <sheetName val="207 HP air-water,new single"/>
-      <sheetName val="207 HP air-water,new apart"/>
-      <sheetName val="207 HP ground-water,ex single"/>
-      <sheetName val="207 HP ground-water,ex apart"/>
-      <sheetName val="207 HP ground-water,new single"/>
-      <sheetName val="207 HP ground-water,new apart"/>
-      <sheetName val="207 HP air-air,ex single"/>
-      <sheetName val="207 HP air-air,new single"/>
-      <sheetName val="207 HP ventilation,new single"/>
-      <sheetName val="207 HP ventilation,new apart"/>
-      <sheetName val="215 Solar heating,ex single"/>
-      <sheetName val="215 Solar heating,ex apart"/>
-      <sheetName val="215 Solar heating,new single"/>
-      <sheetName val="215 Solar heating,new apart"/>
-      <sheetName val="216 Electric heating,new single"/>
-      <sheetName val="216 Electric heating,new apart"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="6">
-          <cell r="B6" t="str">
-            <v>Heat production capacity for one unit [kW_h]</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>Expected share of space heating demand covered by unit [p.u.]</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8" t="str">
-            <v>Expected share of hot tap water demand covered by unit [p.u.]</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9" t="str">
-            <v>Heat efficiency (annual average, net) [p.u.]</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>Auxiliary Electricity consumption [kWh_e/y]</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v>Technical economic lifetime [years]</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13" t="str">
-            <v>Primary regulation (per 30 seconds) [p.u.]</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14" t="str">
-            <v>Secondary regulation (per minute) [p.u.]</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15" t="str">
-            <v>Minimum load (of full load) [p.u.]</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16" t="str">
-            <v>Warm start-up time [hours]</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v>Cold start-up time [hours]</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29" t="str">
-            <v>Fixed O&amp;M (*total) [€/unit/y, 2020]</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30" t="str">
-            <v>Fixed O&amp;M (electricity cost) [€/unit/y, 2020]</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31" t="str">
-            <v>Fixed O&amp;M (other) [€/unit/y, 2020]</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="B32" t="str">
-            <v>Annual O&amp;M (time spent on manual maintenance) [hours/unit/y]</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2258,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:J12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2448,8 +2315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B3:AE18"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2778,7 +2645,7 @@
         <v>204</v>
       </c>
       <c r="H8" s="13">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="I8" s="13">
         <v>1</v>
@@ -3021,7 +2888,7 @@
         <v>248</v>
       </c>
       <c r="H14">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="I14" s="13">
         <v>1</v>
@@ -3169,8 +3036,8 @@
   </sheetPr>
   <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -4954,12 +4821,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B44:M44"/>
-    <mergeCell ref="C3:M3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="B41:M41"/>
-    <mergeCell ref="B43:M43"/>
     <mergeCell ref="B53:M53"/>
     <mergeCell ref="B54:M54"/>
     <mergeCell ref="B55:M55"/>
@@ -4969,6 +4830,12 @@
     <mergeCell ref="B49:M49"/>
     <mergeCell ref="B50:M50"/>
     <mergeCell ref="B51:M51"/>
+    <mergeCell ref="B44:M44"/>
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B41:M41"/>
+    <mergeCell ref="B43:M43"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C3" location="INDEX" display="Heat pumps utilizing industrial waste heat 3 MW" xr:uid="{42BCD51D-8F42-4398-853E-66F8A7B17C5C}"/>
@@ -4985,8 +4852,8 @@
   </sheetPr>
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5137,9 +5004,8 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="105"/>
-      <c r="B8" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B6</f>
-        <v>Heat production capacity for one unit [kW_h]</v>
+      <c r="B8" s="106" t="s">
+        <v>251</v>
       </c>
       <c r="C8" s="107">
         <v>400</v>
@@ -5175,9 +5041,8 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="105"/>
-      <c r="B9" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B7</f>
-        <v>Expected share of space heating demand covered by unit [p.u.]</v>
+      <c r="B9" s="106" t="s">
+        <v>252</v>
       </c>
       <c r="C9" s="108">
         <v>1</v>
@@ -5211,9 +5076,8 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="105"/>
-      <c r="B10" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B8</f>
-        <v>Expected share of hot tap water demand covered by unit [p.u.]</v>
+      <c r="B10" s="106" t="s">
+        <v>253</v>
       </c>
       <c r="C10" s="108">
         <v>1</v>
@@ -5247,9 +5111,8 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="105"/>
-      <c r="B11" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B9</f>
-        <v>Heat efficiency (annual average, net) [p.u.]</v>
+      <c r="B11" s="106" t="s">
+        <v>254</v>
       </c>
       <c r="C11" s="108">
         <v>1</v>
@@ -5285,9 +5148,8 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="105"/>
-      <c r="B12" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B10</f>
-        <v>Auxiliary Electricity consumption [kWh_e/y]</v>
+      <c r="B12" s="106" t="s">
+        <v>255</v>
       </c>
       <c r="C12" s="107">
         <v>600</v>
@@ -5322,9 +5184,8 @@
       <c r="M12" s="107"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B11</f>
-        <v>Technical economic lifetime [years]</v>
+      <c r="B13" s="106" t="s">
+        <v>256</v>
       </c>
       <c r="C13" s="107">
         <v>25</v>
@@ -5377,9 +5238,8 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="105"/>
-      <c r="B15" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B13</f>
-        <v>Primary regulation (per 30 seconds) [p.u.]</v>
+      <c r="B15" s="106" t="s">
+        <v>257</v>
       </c>
       <c r="C15" s="107"/>
       <c r="D15" s="107"/>
@@ -5395,9 +5255,8 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="105"/>
-      <c r="B16" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B14</f>
-        <v>Secondary regulation (per minute) [p.u.]</v>
+      <c r="B16" s="106" t="s">
+        <v>258</v>
       </c>
       <c r="C16" s="107"/>
       <c r="D16" s="107"/>
@@ -5413,9 +5272,8 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="105"/>
-      <c r="B17" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B15</f>
-        <v>Minimum load (of full load) [p.u.]</v>
+      <c r="B17" s="106" t="s">
+        <v>259</v>
       </c>
       <c r="C17" s="107"/>
       <c r="D17" s="107"/>
@@ -5431,9 +5289,8 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="105"/>
-      <c r="B18" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B16</f>
-        <v>Warm start-up time [hours]</v>
+      <c r="B18" s="106" t="s">
+        <v>260</v>
       </c>
       <c r="C18" s="107"/>
       <c r="D18" s="107"/>
@@ -5449,9 +5306,8 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="105"/>
-      <c r="B19" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B17</f>
-        <v>Cold start-up time [hours]</v>
+      <c r="B19" s="106" t="s">
+        <v>261</v>
       </c>
       <c r="C19" s="107"/>
       <c r="D19" s="107"/>
@@ -5728,9 +5584,8 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="105"/>
-      <c r="B31" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B29</f>
-        <v>Fixed O&amp;M (*total) [€/unit/y, 2020]</v>
+      <c r="B31" s="106" t="s">
+        <v>262</v>
       </c>
       <c r="C31" s="113">
         <v>140.4</v>
@@ -5765,9 +5620,8 @@
       <c r="M31" s="107"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B32" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B30</f>
-        <v>Fixed O&amp;M (electricity cost) [€/unit/y, 2020]</v>
+      <c r="B32" s="106" t="s">
+        <v>263</v>
       </c>
       <c r="C32" s="114">
         <v>41.400000000000006</v>
@@ -5800,9 +5654,8 @@
       <c r="M32" s="108"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B33" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B31</f>
-        <v>Fixed O&amp;M (other) [€/unit/y, 2020]</v>
+      <c r="B33" s="106" t="s">
+        <v>264</v>
       </c>
       <c r="C33" s="115">
         <v>99</v>
@@ -5836,9 +5689,8 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="105"/>
-      <c r="B34" s="106" t="str">
-        <f>'[1]201 Oil boiler, ex single'!B32</f>
-        <v>Annual O&amp;M (time spent on manual maintenance) [hours/unit/y]</v>
+      <c r="B34" s="106" t="s">
+        <v>265</v>
       </c>
       <c r="C34" s="113">
         <v>0</v>

</xml_diff>